<commit_message>
day 2 new male pair
</commit_message>
<xml_diff>
--- a/Training_weight_record.xlsx
+++ b/Training_weight_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjpc/Documents/Internship_notes_UO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B310E092-4873-5E40-9954-EC5D992B925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ABDF21-29F6-514A-8F0D-6BE8AA11AB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{F0298443-DE12-0040-8AE0-BF13E0A12569}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -63,12 +63,36 @@
   </si>
   <si>
     <t>Day 3 (2023-02-24)</t>
+  </si>
+  <si>
+    <t>Day 4 (2023-02-25)</t>
+  </si>
+  <si>
+    <t>coop014</t>
+  </si>
+  <si>
+    <t>coop015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Day 1 (2023-03-02)</t>
+  </si>
+  <si>
+    <t>Day 2 (2023-03-03)</t>
+  </si>
+  <si>
+    <t>Day 3 (2023-03-04)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,8 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,18 +446,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8FED73-E9D9-484C-95B2-9E382CC7B142}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,10 +473,16 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,11 +496,18 @@
         <v>20.399999999999999</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(B2:D2)</f>
-        <v>20.866666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20.8</v>
+      </c>
+      <c r="F2" s="1">
+        <f>AVERAGE(B2:E2)</f>
+        <v>20.85</v>
+      </c>
+      <c r="G2" s="1">
+        <f>F2*0.8</f>
+        <v>16.680000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -480,11 +521,18 @@
         <v>20.3</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E5" si="0">AVERAGE(B3:D3)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <f>AVERAGE(B3:E3)</f>
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G5" si="0">F3*0.8</f>
+        <v>16.080000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,11 +546,18 @@
         <v>23.4</v>
       </c>
       <c r="E4">
+        <v>23.5</v>
+      </c>
+      <c r="F4" s="1">
+        <f>AVERAGE(B4:E4)</f>
+        <v>23.25</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>23.166666666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -516,8 +571,53 @@
         <v>24.8</v>
       </c>
       <c r="E5">
+        <v>25.1</v>
+      </c>
+      <c r="F5" s="1">
+        <f>AVERAGE(B5:E5)</f>
+        <v>24.774999999999999</v>
+      </c>
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>24.666666666666668</v>
+        <v>19.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>27.8</v>
+      </c>
+      <c r="C7">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>29.2</v>
+      </c>
+      <c r="C8">
+        <v>29.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 3 new male pair
</commit_message>
<xml_diff>
--- a/Training_weight_record.xlsx
+++ b/Training_weight_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjpc/Documents/Internship_notes_UO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ABDF21-29F6-514A-8F0D-6BE8AA11AB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F534096-84DB-644F-B544-12417CBE5D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{F0298443-DE12-0040-8AE0-BF13E0A12569}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +528,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G5" si="0">F3*0.8</f>
+        <f t="shared" ref="G3:G8" si="0">F3*0.8</f>
         <v>16.080000000000002</v>
       </c>
     </row>
@@ -608,6 +608,17 @@
       <c r="C7">
         <v>28.1</v>
       </c>
+      <c r="D7">
+        <v>28.2</v>
+      </c>
+      <c r="F7" s="1">
+        <f>AVERAGE(B7:D7)</f>
+        <v>28.033333333333335</v>
+      </c>
+      <c r="G7" s="1">
+        <f>F7*0.8</f>
+        <v>22.426666666666669</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -618,6 +629,17 @@
       </c>
       <c r="C8">
         <v>29.1</v>
+      </c>
+      <c r="D8">
+        <v>29.4</v>
+      </c>
+      <c r="F8" s="1">
+        <f>AVERAGE(B8:D8)</f>
+        <v>29.233333333333331</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>23.386666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>